<commit_message>
bug fixed in payment filtering
</commit_message>
<xml_diff>
--- a/src/assets/images/payments.xlsx
+++ b/src/assets/images/payments.xlsx
@@ -1,19 +1,71 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\angular projects\go-fund-me\src\assets\images\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2458B3-CDAD-4D20-BA99-AB3F3679E72B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>Bank name</t>
+  </si>
+  <si>
+    <t>Bank account no.</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Fundraiser ID</t>
+  </si>
+  <si>
+    <t>Fasikaw</t>
+  </si>
+  <si>
+    <t>Kindye</t>
+  </si>
+  <si>
+    <t>Cvg</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>6155f2754bde6bb71afe5f7a</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -50,6 +102,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -374,14 +434,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError sqref="A1:F2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>